<commit_message>
Criação da Classe LeitorJson
</commit_message>
<xml_diff>
--- a/projeto-base-selenium/src/test/java/SISTEMA/transacoes/cadastro_basico/moedas/MoedasTest.xlsx
+++ b/projeto-base-selenium/src/test/java/SISTEMA/transacoes/cadastro_basico/moedas/MoedasTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\ws_robo\projeto-base-selenium\src\test\java\SISTEMA\cadastro_basico\moedas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipem.medeiros\Documents\cursos\SELENIUM\base-selenio\projeto-base-selenium\src\test\java\SISTEMA\transacoes\cadastro_basico\moedas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>